<commit_message>
prog1 configurations; added cpu version
</commit_message>
<xml_diff>
--- a/CLE3_T3G5/configs_prog1.xlsx
+++ b/CLE3_T3G5/configs_prog1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14joa\Faculdade\UA\Semestre2\CLE\Assignment\CLE_2022_2023\CLE3_T3G5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis1\Documents\ubuntu_shared\CLE\CLE_2022_2023\CLE3_T3G5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9273E352-F384-4A3D-8764-54D6C12D395D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72870622-34A4-457A-A52B-BE03F37AA9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7D3F91F4-B404-421F-A1CF-5244EAEDD666}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D3F91F4-B404-421F-A1CF-5244EAEDD666}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="8">
   <si>
     <t>blockDimX</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,26 +277,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -303,9 +299,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -622,22 +615,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8229D8-8ECD-4077-BCFB-46B3A1A858CA}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="25"/>
-    <col min="2" max="3" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="22"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -655,14 +648,14 @@
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -685,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -708,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>4</v>
       </c>
@@ -731,7 +724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>8</v>
       </c>
@@ -754,7 +747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>16</v>
       </c>
@@ -777,7 +770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>1</v>
       </c>
@@ -800,7 +793,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -823,7 +816,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>2</v>
       </c>
@@ -846,7 +839,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>2</v>
       </c>
@@ -869,7 +862,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>1</v>
       </c>
@@ -892,7 +885,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>1</v>
       </c>
@@ -909,7 +902,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>1</v>
       </c>
@@ -926,7 +919,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>1</v>
       </c>
@@ -943,9 +936,9 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -964,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>1</v>
       </c>
@@ -981,7 +974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -998,7 +991,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>4</v>
       </c>
@@ -1015,7 +1008,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>8</v>
       </c>
@@ -1032,7 +1025,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>1</v>
       </c>
@@ -1049,7 +1042,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>1</v>
       </c>
@@ -1066,7 +1059,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>1</v>
       </c>
@@ -1083,7 +1076,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="12">
         <v>2</v>
       </c>
@@ -1100,7 +1093,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>1</v>
       </c>
@@ -1117,7 +1110,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>1</v>
       </c>
@@ -1134,7 +1127,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
         <v>1</v>
       </c>
@@ -1151,7 +1144,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <v>1</v>
       </c>
@@ -1168,7 +1161,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
         <v>1</v>
       </c>
@@ -1185,9 +1178,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="25">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22">
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1206,7 +1199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>1</v>
       </c>
@@ -1223,7 +1216,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
         <v>4</v>
       </c>
@@ -1240,7 +1233,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="7">
         <v>8</v>
       </c>
@@ -1257,7 +1250,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="7">
         <v>1</v>
       </c>
@@ -1274,11 +1267,11 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="16">
-        <v>1</v>
-      </c>
-      <c r="C37" s="16">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
+        <v>1</v>
+      </c>
+      <c r="C37" s="15">
         <v>2</v>
       </c>
       <c r="D37" s="5">
@@ -1291,7 +1284,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="7">
         <v>2</v>
       </c>
@@ -1308,7 +1301,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12">
         <v>4</v>
       </c>
@@ -1325,24 +1318,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="17">
-        <v>1</v>
-      </c>
-      <c r="C40" s="17">
-        <v>2</v>
-      </c>
-      <c r="D40" s="17">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="16">
+        <v>1</v>
+      </c>
+      <c r="C40" s="16">
+        <v>2</v>
+      </c>
+      <c r="D40" s="16">
         <v>32</v>
       </c>
-      <c r="E40" s="17">
-        <v>4</v>
-      </c>
-      <c r="F40" s="17">
+      <c r="E40" s="16">
+        <v>4</v>
+      </c>
+      <c r="F40" s="16">
         <v>13.7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="7">
         <v>1</v>
       </c>
@@ -1359,7 +1352,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="7">
         <v>1</v>
       </c>
@@ -1376,7 +1369,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="7">
         <v>1</v>
       </c>
@@ -1393,15 +1386,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="25">
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="22">
         <v>3</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1419,9 +1412,8 @@
       <c r="F45" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H45" s="18"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>1</v>
       </c>
@@ -1438,7 +1430,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="5">
         <v>2</v>
       </c>
@@ -1455,11 +1447,11 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="20">
-        <v>1</v>
-      </c>
-      <c r="C48" s="20">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="18">
+        <v>1</v>
+      </c>
+      <c r="C48" s="18">
         <v>2</v>
       </c>
       <c r="D48" s="13">
@@ -1472,7 +1464,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="12">
         <v>2</v>
       </c>
@@ -1489,11 +1481,11 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="21">
-        <v>1</v>
-      </c>
-      <c r="C50" s="21">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="4">
         <v>2</v>
       </c>
       <c r="D50" s="4">
@@ -1506,7 +1498,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
         <v>1</v>
       </c>
@@ -1523,7 +1515,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="6">
         <v>1</v>
       </c>
@@ -1540,16 +1532,15 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="26"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-    </row>
-    <row r="54" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="25">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="22">
         <v>4</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -1568,24 +1559,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="23">
-        <v>1</v>
-      </c>
-      <c r="C55" s="23">
-        <v>1</v>
-      </c>
-      <c r="D55" s="24">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="20">
+        <v>1</v>
+      </c>
+      <c r="C55" s="20">
+        <v>1</v>
+      </c>
+      <c r="D55" s="21">
         <v>64</v>
       </c>
-      <c r="E55" s="24">
-        <v>1</v>
-      </c>
-      <c r="F55" s="24">
+      <c r="E55" s="21">
+        <v>1</v>
+      </c>
+      <c r="F55" s="21">
         <v>42.8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" s="5">
         <v>2</v>
       </c>
@@ -1602,7 +1593,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="9">
         <v>1</v>
       </c>
@@ -1619,7 +1610,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="12">
         <v>1</v>
       </c>
@@ -1636,7 +1627,7 @@
         <v>55.4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" s="10">
         <v>1</v>
       </c>
@@ -1653,7 +1644,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="7">
         <v>1</v>
       </c>
@@ -1670,7 +1661,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="7">
         <v>1</v>
       </c>
@@ -1687,7 +1678,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" s="7">
         <v>1</v>
       </c>
@@ -1704,9 +1695,9 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="25">
+    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="22">
         <v>5</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -1725,11 +1716,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="23">
-        <v>1</v>
-      </c>
-      <c r="C65" s="23">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="20">
+        <v>1</v>
+      </c>
+      <c r="C65" s="20">
         <v>1</v>
       </c>
       <c r="D65" s="4">
@@ -1742,7 +1733,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" s="5">
         <v>2</v>
       </c>
@@ -1759,7 +1750,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" s="9">
         <v>1</v>
       </c>
@@ -1776,7 +1767,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="12">
         <v>1</v>
       </c>
@@ -1793,7 +1784,7 @@
         <v>87.6</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="10">
         <v>1</v>
       </c>
@@ -1810,7 +1801,7 @@
         <v>84.4</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
         <v>1</v>
       </c>
@@ -1827,7 +1818,7 @@
         <v>84.4</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" s="6">
         <v>1</v>
       </c>
@@ -1844,7 +1835,521 @@
         <v>84.3</v>
       </c>
     </row>
+    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="22">
+        <v>6</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="20">
+        <v>1</v>
+      </c>
+      <c r="C74" s="20">
+        <v>1</v>
+      </c>
+      <c r="D74" s="4">
+        <v>16</v>
+      </c>
+      <c r="E74" s="4">
+        <v>1</v>
+      </c>
+      <c r="F74" s="4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="5">
+        <v>2</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5">
+        <v>8</v>
+      </c>
+      <c r="E75" s="5">
+        <v>1</v>
+      </c>
+      <c r="F75" s="5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="9">
+        <v>1</v>
+      </c>
+      <c r="C76" s="9">
+        <v>2</v>
+      </c>
+      <c r="D76" s="13">
+        <v>8</v>
+      </c>
+      <c r="E76" s="13">
+        <v>1</v>
+      </c>
+      <c r="F76" s="13">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="12">
+        <v>1</v>
+      </c>
+      <c r="C77" s="12">
+        <v>4</v>
+      </c>
+      <c r="D77" s="14">
+        <v>4</v>
+      </c>
+      <c r="E77" s="14">
+        <v>1</v>
+      </c>
+      <c r="F77" s="14">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="10">
+        <v>1</v>
+      </c>
+      <c r="C78" s="10">
+        <v>1</v>
+      </c>
+      <c r="D78" s="10">
+        <v>4</v>
+      </c>
+      <c r="E78" s="10">
+        <v>4</v>
+      </c>
+      <c r="F78" s="10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="7">
+        <v>1</v>
+      </c>
+      <c r="C79" s="7">
+        <v>1</v>
+      </c>
+      <c r="D79" s="7">
+        <v>2</v>
+      </c>
+      <c r="E79" s="7">
+        <v>8</v>
+      </c>
+      <c r="F79" s="7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="6">
+        <v>1</v>
+      </c>
+      <c r="C80" s="6">
+        <v>1</v>
+      </c>
+      <c r="D80" s="6">
+        <v>1</v>
+      </c>
+      <c r="E80" s="6">
+        <v>16</v>
+      </c>
+      <c r="F80" s="6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="22">
+        <v>7</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="20">
+        <v>1</v>
+      </c>
+      <c r="C83" s="20">
+        <v>1</v>
+      </c>
+      <c r="D83" s="4">
+        <v>8</v>
+      </c>
+      <c r="E83" s="4">
+        <v>1</v>
+      </c>
+      <c r="F83" s="4">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="5">
+        <v>2</v>
+      </c>
+      <c r="C84" s="5">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5">
+        <v>4</v>
+      </c>
+      <c r="E84" s="5">
+        <v>1</v>
+      </c>
+      <c r="F84" s="5">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="9">
+        <v>1</v>
+      </c>
+      <c r="C85" s="9">
+        <v>2</v>
+      </c>
+      <c r="D85" s="13">
+        <v>4</v>
+      </c>
+      <c r="E85" s="13">
+        <v>1</v>
+      </c>
+      <c r="F85" s="13">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="12">
+        <v>1</v>
+      </c>
+      <c r="C86" s="12">
+        <v>4</v>
+      </c>
+      <c r="D86" s="14">
+        <v>2</v>
+      </c>
+      <c r="E86" s="14">
+        <v>1</v>
+      </c>
+      <c r="F86" s="14">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="10">
+        <v>1</v>
+      </c>
+      <c r="C87" s="10">
+        <v>1</v>
+      </c>
+      <c r="D87" s="10">
+        <v>4</v>
+      </c>
+      <c r="E87" s="10">
+        <v>2</v>
+      </c>
+      <c r="F87" s="10">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="6">
+        <v>1</v>
+      </c>
+      <c r="C88" s="6">
+        <v>1</v>
+      </c>
+      <c r="D88" s="6">
+        <v>2</v>
+      </c>
+      <c r="E88" s="6">
+        <v>4</v>
+      </c>
+      <c r="F88" s="6">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="7">
+        <v>1</v>
+      </c>
+      <c r="C89" s="7">
+        <v>1</v>
+      </c>
+      <c r="D89" s="7">
+        <v>1</v>
+      </c>
+      <c r="E89" s="7">
+        <v>8</v>
+      </c>
+      <c r="F89" s="7">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="22">
+        <v>8</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="20">
+        <v>1</v>
+      </c>
+      <c r="C92" s="20">
+        <v>1</v>
+      </c>
+      <c r="D92" s="4">
+        <v>4</v>
+      </c>
+      <c r="E92" s="4">
+        <v>1</v>
+      </c>
+      <c r="F92" s="4">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="5">
+        <v>2</v>
+      </c>
+      <c r="C93" s="5">
+        <v>1</v>
+      </c>
+      <c r="D93" s="5">
+        <v>2</v>
+      </c>
+      <c r="E93" s="5">
+        <v>1</v>
+      </c>
+      <c r="F93" s="5">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="12">
+        <v>1</v>
+      </c>
+      <c r="C94" s="12">
+        <v>2</v>
+      </c>
+      <c r="D94" s="14">
+        <v>2</v>
+      </c>
+      <c r="E94" s="14">
+        <v>1</v>
+      </c>
+      <c r="F94" s="14">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="21">
+        <v>1</v>
+      </c>
+      <c r="C95" s="21">
+        <v>1</v>
+      </c>
+      <c r="D95" s="21">
+        <v>2</v>
+      </c>
+      <c r="E95" s="21">
+        <v>2</v>
+      </c>
+      <c r="F95" s="21">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="7">
+        <v>1</v>
+      </c>
+      <c r="C96" s="7">
+        <v>1</v>
+      </c>
+      <c r="D96" s="7">
+        <v>1</v>
+      </c>
+      <c r="E96" s="7">
+        <v>4</v>
+      </c>
+      <c r="F96" s="7">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="22">
+        <v>9</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="20">
+        <v>1</v>
+      </c>
+      <c r="C99" s="20">
+        <v>1</v>
+      </c>
+      <c r="D99" s="4">
+        <v>2</v>
+      </c>
+      <c r="E99" s="4">
+        <v>1</v>
+      </c>
+      <c r="F99" s="4">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="5">
+        <v>2</v>
+      </c>
+      <c r="C100" s="5">
+        <v>1</v>
+      </c>
+      <c r="D100" s="5">
+        <v>1</v>
+      </c>
+      <c r="E100" s="5">
+        <v>1</v>
+      </c>
+      <c r="F100" s="5">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="12">
+        <v>1</v>
+      </c>
+      <c r="C101" s="12">
+        <v>2</v>
+      </c>
+      <c r="D101" s="14">
+        <v>1</v>
+      </c>
+      <c r="E101" s="14">
+        <v>1</v>
+      </c>
+      <c r="F101" s="14">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="21">
+        <v>1</v>
+      </c>
+      <c r="C102" s="21">
+        <v>1</v>
+      </c>
+      <c r="D102" s="21">
+        <v>1</v>
+      </c>
+      <c r="E102" s="21">
+        <v>2</v>
+      </c>
+      <c r="F102" s="21">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="22">
+        <v>10</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B105" s="21">
+        <v>1</v>
+      </c>
+      <c r="C105" s="21">
+        <v>1</v>
+      </c>
+      <c r="D105" s="21">
+        <v>1</v>
+      </c>
+      <c r="E105" s="21">
+        <v>1</v>
+      </c>
+      <c r="F105" s="21">
+        <v>2.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>